<commit_message>
testing classification models - giving me one correct winner
Maverick winner
</commit_message>
<xml_diff>
--- a/predictions.xlsx
+++ b/predictions.xlsx
@@ -3508,7 +3508,7 @@
         <v>0</v>
       </c>
       <c r="AW20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -4551,7 +4551,7 @@
         <v>0</v>
       </c>
       <c r="AW27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -6339,7 +6339,7 @@
         <v>0</v>
       </c>
       <c r="AW39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -6935,7 +6935,7 @@
         <v>0</v>
       </c>
       <c r="AW43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -7084,7 +7084,7 @@
         <v>0</v>
       </c>
       <c r="AW44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">

</xml_diff>